<commit_message>
string to int and float
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,73 +434,124 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>키워드</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>상품수</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>한달검색수</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>6개월매출</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>6개월판매량</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>평균가격</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>경쟁강도</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>경쟁강도지표</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>홍당무</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>수박</t>
+          <t>493</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>80,741만원</t>
+          <t>5567</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>35,194개</t>
+          <t>4500</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>19,800원</t>
+          <t>24310</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>268,391개</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>186,000회</t>
-        </is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3.93</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.44</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>아주좋음</t>
+          <t>좋음</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>당근</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>53129</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>62581</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>11800</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>455787</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>78300</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>좋음</t>
         </is>
       </c>
     </row>

</xml_diff>